<commit_message>
added CI accuracy and duration
</commit_message>
<xml_diff>
--- a/Sonuçlar.xlsx
+++ b/Sonuçlar.xlsx
@@ -8,24 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\semiha\Desktop\Master\Wordlefastapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD07D71E-5732-413C-87EB-BC369CBD045C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15FE709-1038-425B-ACBE-174AA065B1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="3" xr2:uid="{63F9D13E-EE14-445C-97E3-166A902E54E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{63F9D13E-EE14-445C-97E3-166A902E54E2}"/>
   </bookViews>
   <sheets>
-    <sheet name="game_level_summary" sheetId="2" r:id="rId1"/>
-    <sheet name="6 dan büyük başarısızlık değerl" sheetId="1" r:id="rId2"/>
-    <sheet name="3 yöntem başarı -başarısızlık " sheetId="4" r:id="rId3"/>
-    <sheet name="top5_kelime_frekans (2)" sheetId="7" r:id="rId4"/>
+    <sheet name="LSTM ve Hibrit sonucları" sheetId="2" r:id="rId1"/>
+    <sheet name="3 yöntem başarı -başarısızlık " sheetId="4" r:id="rId2"/>
+    <sheet name="top5_kelime_frekans (2)" sheetId="7" r:id="rId3"/>
+    <sheet name="Yöntem Hesaplama Süreleri" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="2" hidden="1">'3 yöntem başarı -başarısızlık '!$A$1:$D$4</definedName>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">game_level_summary!$A$1:$C$5</definedName>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'top5_kelime_frekans (2)'!$A$1:$D$16</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'3 yöntem başarı -başarısızlık '!$A$1:$E$4</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'LSTM ve Hibrit sonucları'!$A$1:$C$5</definedName>
+    <definedName name="ExternalData_1" localSheetId="2" hidden="1">'top5_kelime_frekans (2)'!$A$1:$D$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="44" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>Method</t>
   </si>
@@ -167,12 +167,78 @@
   <si>
     <t>Sum of Frequency</t>
   </si>
+  <si>
+    <t>95% CI</t>
+  </si>
+  <si>
+    <t>0.983 – 0.995</t>
+  </si>
+  <si>
+    <t>0.939 – 0.965</t>
+  </si>
+  <si>
+    <t>0.906 – 0.940</t>
+  </si>
+  <si>
+    <t>Yöntem</t>
+  </si>
+  <si>
+    <t>Ortalama süre (yaklaşık)</t>
+  </si>
+  <si>
+    <t>İlk adım süresi</t>
+  </si>
+  <si>
+    <t>Sonraki adımlar</t>
+  </si>
+  <si>
+    <t>Değerlendirme</t>
+  </si>
+  <si>
+    <t>~10 s (tahmini)</t>
+  </si>
+  <si>
+    <t>~25 s</t>
+  </si>
+  <si>
+    <t>&lt;1 s</t>
+  </si>
+  <si>
+    <t>En doğru ama ağır</t>
+  </si>
+  <si>
+    <t>Hybrid Prediction</t>
+  </si>
+  <si>
+    <t>~0.1–0.3 s</t>
+  </si>
+  <si>
+    <t>0.1–0.3 s</t>
+  </si>
+  <si>
+    <t>0.002–0.01 s</t>
+  </si>
+  <si>
+    <t>~0.01–0.02 s</t>
+  </si>
+  <si>
+    <t>0.015 s</t>
+  </si>
+  <si>
+    <t>~0.001 s</t>
+  </si>
+  <si>
+    <t>Çok hızlı ama doğruluk düşük</t>
+  </si>
+  <si>
+    <t>Hızlı ve süresi iyi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,23 +247,42 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -220,22 +305,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -243,11 +334,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -329,7 +473,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>game_level_summary!$B$1</c:f>
+              <c:f>'LSTM ve Hibrit sonucları'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -408,7 +552,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>game_level_summary!$A$2:$A$5</c:f>
+              <c:f>'LSTM ve Hibrit sonucları'!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -428,7 +572,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>game_level_summary!$B$2:$B$5</c:f>
+              <c:f>'LSTM ve Hibrit sonucları'!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -682,7 +826,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>game_level_summary!$C$1</c:f>
+              <c:f>'LSTM ve Hibrit sonucları'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -703,7 +847,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>game_level_summary!$A$2:$A$5</c:f>
+              <c:f>'LSTM ve Hibrit sonucları'!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -723,7 +867,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>game_level_summary!$C$2:$C$5</c:f>
+              <c:f>'LSTM ve Hibrit sonucları'!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1011,7 +1155,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'3 yöntem başarı -başarısızlık '!$C$1</c:f>
+              <c:f>'3 yöntem başarı -başarısızlık '!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1049,7 +1193,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3 yöntem başarı -başarısızlık '!$C$2:$C$4</c:f>
+              <c:f>'3 yöntem başarı -başarısızlık '!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -4560,7 +4704,7 @@
       <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -4775,7 +4919,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A8FC17E-D99D-48FA-B627-9356D8EFB760}" name="PivotTable20" cacheId="44" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A8FC17E-D99D-48FA-B627-9356D8EFB760}" name="PivotTable20" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="H1:L18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -4946,10 +5090,11 @@
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="2" xr16:uid="{37B661EE-7C1B-4CAE-A12A-D28FD65A3397}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="5">
-    <queryTableFields count="4">
+  <queryTableRefresh nextId="6">
+    <queryTableFields count="5">
       <queryTableField id="1" name="Method" tableColumnId="1"/>
       <queryTableField id="2" name="Accuracy" tableColumnId="2"/>
+      <queryTableField id="5" dataBound="0" tableColumnId="5"/>
       <queryTableField id="4" dataBound="0" tableColumnId="4"/>
       <queryTableField id="3" name="Average Step" tableColumnId="3"/>
     </queryTableFields>
@@ -4974,7 +5119,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8821AB12-03D4-4496-88CD-20D4E4C5F812}" name="game_level_summary" displayName="game_level_summary" ref="A1:C5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:C5" xr:uid="{8821AB12-03D4-4496-88CD-20D4E4C5F812}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3B9B2C89-1345-4628-B3DC-E82483513E33}" uniqueName="1" name="Method" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{3B9B2C89-1345-4628-B3DC-E82483513E33}" uniqueName="1" name="Method" queryTableFieldId="1" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{E5244782-F54C-40FF-8C3C-6D23309E1279}" uniqueName="2" name="Accuracy" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{BBFAEF27-04C3-4509-8ABA-985CCB29372E}" uniqueName="3" name="Average Step" queryTableFieldId="3"/>
   </tableColumns>
@@ -4983,11 +5128,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{911DD9C6-E82D-46D0-B30D-7E05C6205341}" name="game_level_summary__2" displayName="game_level_summary__2" ref="A1:D4" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{911DD9C6-E82D-46D0-B30D-7E05C6205341}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0D733A0F-42AF-43AA-82C2-D3B872D29B93}" uniqueName="1" name="Method" queryTableFieldId="1" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{911DD9C6-E82D-46D0-B30D-7E05C6205341}" name="game_level_summary__2" displayName="game_level_summary__2" ref="A1:E4" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:E4" xr:uid="{911DD9C6-E82D-46D0-B30D-7E05C6205341}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{0D733A0F-42AF-43AA-82C2-D3B872D29B93}" uniqueName="1" name="Method" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{6A609DB8-87D0-416D-ACEF-7F33A4F2399D}" uniqueName="2" name="Accuracy" queryTableFieldId="2"/>
+    <tableColumn id="5" xr3:uid="{47024F76-63EC-4203-855C-662D2C275F5D}" uniqueName="5" name="95% CI" queryTableFieldId="5" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{775C0522-37F4-47A7-90A5-0D4559F507E1}" uniqueName="4" name="Failure / Unsuccessful prediction" queryTableFieldId="4"/>
     <tableColumn id="3" xr3:uid="{4F6B3A08-82A6-46A4-9823-E8CD284DACA5}" uniqueName="3" name="Average Step" queryTableFieldId="3"/>
   </tableColumns>
@@ -4999,8 +5145,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6D344A28-BF22-497D-8833-7D37DD862E42}" name="top5_kelime_frekans" displayName="top5_kelime_frekans" ref="A1:D16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D16" xr:uid="{6D344A28-BF22-497D-8833-7D37DD862E42}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C85F433D-20C4-491A-AC7F-262BFC54FB6E}" uniqueName="1" name="WORD" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{D092B43A-519D-4C67-9842-45AF54BC8A80}" uniqueName="2" name="METHOD" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C85F433D-20C4-491A-AC7F-262BFC54FB6E}" uniqueName="1" name="WORD" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D092B43A-519D-4C67-9842-45AF54BC8A80}" uniqueName="2" name="METHOD" queryTableFieldId="2" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{669F93BB-6FA3-4F99-9AB9-EE776EE0783C}" uniqueName="3" name="COUNT" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{8EF558D7-C304-4C6C-86EC-66DE4E5AAF35}" uniqueName="4" name="Frequency" queryTableFieldId="4"/>
   </tableColumns>
@@ -5325,10 +5471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830CC495-02BC-4D8D-9F51-193FD6E3DACA}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5336,9 +5482,10 @@
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5348,9 +5495,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
@@ -5359,9 +5511,14 @@
       <c r="C2">
         <v>3.9020807833537332</v>
       </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
@@ -5370,9 +5527,14 @@
       <c r="C3">
         <v>3.8331332533013205</v>
       </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
@@ -5381,9 +5543,14 @@
       <c r="C4">
         <v>3.4100106496272629</v>
       </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
@@ -5403,132 +5570,137 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4ABBA00-9BF3-4255-A29C-105BDF6EE7E0}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1353B78-B4B3-46D5-8641-3975871E4062}">
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5">
-        <v>77</v>
-      </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5">
-        <v>48</v>
-      </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="5">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1353B78-B4B3-46D5-8641-3975871E4062}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" customWidth="1"/>
+    <col min="12" max="15" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
+      <c r="H1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2">
         <v>0.98899999999999999</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>3.1253791708796763</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1">
+        <v>77</v>
+      </c>
+      <c r="K2" s="6"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3">
         <v>0.95199999999999996</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3.3413865546218489</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1">
+        <v>48</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
         <v>0.92300000000000004</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>3.533044420368364</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>11</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5539,11 +5711,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA6FFD9-46D6-4CCC-AB94-EED19543B65C}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
@@ -5577,18 +5749,18 @@
       <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2">
@@ -5597,7 +5769,7 @@
       <c r="D2">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="2" t="s">
         <v>27</v>
       </c>
       <c r="I2" t="s">
@@ -5614,10 +5786,10 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3">
@@ -5626,23 +5798,21 @@
       <c r="D3">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1">
+      <c r="K3">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3">
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4">
@@ -5651,23 +5821,21 @@
       <c r="D4">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1">
+      <c r="K4">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4">
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5">
@@ -5676,23 +5844,21 @@
       <c r="D5">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1">
+      <c r="J5">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1">
+      <c r="L5">
         <v>6.4999999999999997E-3</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6">
@@ -5701,23 +5867,21 @@
       <c r="D6">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1">
+      <c r="J6">
         <v>3.3E-3</v>
       </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1">
+      <c r="L6">
         <v>3.3E-3</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -5726,23 +5890,21 @@
       <c r="D7">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1">
+      <c r="J7">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1">
+      <c r="L7">
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8">
@@ -5751,23 +5913,21 @@
       <c r="D8">
         <v>5.3E-3</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1">
+      <c r="J8">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1">
+      <c r="L8">
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9">
@@ -5776,23 +5936,21 @@
       <c r="D9">
         <v>3.3E-3</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1">
+      <c r="J9">
         <v>5.3E-3</v>
       </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1">
+      <c r="L9">
         <v>5.3E-3</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10">
@@ -5801,23 +5959,21 @@
       <c r="D10">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1">
+      <c r="L10">
         <v>6.7000000000000002E-3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11">
@@ -5826,23 +5982,21 @@
       <c r="D11">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1">
+      <c r="L11">
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12">
@@ -5851,23 +6005,21 @@
       <c r="D12">
         <v>7.3000000000000001E-3</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1">
+      <c r="L12">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13">
@@ -5876,23 +6028,21 @@
       <c r="D13">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1">
+      <c r="L13">
         <v>6.7000000000000002E-3</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14">
@@ -5901,23 +6051,21 @@
       <c r="D14">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14">
         <v>7.3000000000000001E-3</v>
       </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1">
+      <c r="L14">
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="C15">
@@ -5926,23 +6074,21 @@
       <c r="D15">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1">
+      <c r="K15">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15">
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16">
@@ -5951,45 +6097,41 @@
       <c r="D16">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1">
+      <c r="K16">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16">
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
     <row r="17" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1">
+      <c r="K17">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L17">
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
     <row r="18" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18">
         <v>2.8400000000000002E-2</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18">
         <v>2.0500000000000001E-2</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18">
         <v>6.0999999999999995E-3</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L18">
         <v>5.5E-2</v>
       </c>
     </row>
@@ -5999,6 +6141,94 @@
   <tableParts count="1">
     <tablePart r:id="rId3"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CECDB2B-7DD3-4AD6-BEFE-ED1432978665}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>